<commit_message>
mais um pushzinho de cria
</commit_message>
<xml_diff>
--- a/Mul-TP1.xlsx
+++ b/Mul-TP1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\3ºSemestre\Multimedia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF94109-D92F-4CEF-9D4D-8C4B98062449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8CF1313-7A3A-459B-83EA-3E0FB3C5F1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9D918505-94C9-48F7-8700-9E7130F13C1A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>B</t>
   </si>
@@ -56,10 +56,46 @@
     <t>nature</t>
   </si>
   <si>
-    <t>Qualidade</t>
-  </si>
-  <si>
     <t>Compressão</t>
+  </si>
+  <si>
+    <t>15.36:1</t>
+  </si>
+  <si>
+    <t>22.88:1</t>
+  </si>
+  <si>
+    <t>35.16:1</t>
+  </si>
+  <si>
+    <t>49.47:1</t>
+  </si>
+  <si>
+    <t>64.79:1</t>
+  </si>
+  <si>
+    <t>87.16:1</t>
+  </si>
+  <si>
+    <t>14.01:1</t>
+  </si>
+  <si>
+    <t>18.55:1</t>
+  </si>
+  <si>
+    <t>48.04:1</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Qualidade-Subjetiva</t>
   </si>
 </sst>
 </file>
@@ -100,7 +136,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,21 +473,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CD8E1A0-40AD-41D1-AB95-ABCAAE3579E4}">
-  <dimension ref="C5:L8"/>
+  <dimension ref="C5:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" activeCellId="1" sqref="F8 H20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="151" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
@@ -462,7 +500,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>0</v>
@@ -474,29 +512,83 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="I8" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>